<commit_message>
Expand and improve documentation for core analysis functions
Enhanced and extended the documentation for key analysis and data handling functions, including CopyDataModel, DiagramFP, ExergyAnalysis, ExportResults, ImportData, ImportDataModel, and ListResultTables. The updates provide detailed usage instructions, comprehensive examples, workflow integration notes, error handling guidance, and platform compatibility information. These improvements make the functions more accessible and user-friendly for both new and experienced users, and clarify the purpose and capabilities of each function. No changes were made to the computational logic or outputs.
</commit_message>
<xml_diff>
--- a/DocUtils/Contents.xlsx
+++ b/DocUtils/Contents.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ctorr\Documents\Proyectos\TaesLab\DocUtils\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79AA3A4A-4356-46A1-9412-B99684549AF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC0D3A1D-56F2-4747-A295-C7E1E38A0AD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Index" sheetId="9" r:id="rId1"/>
@@ -120,60 +120,18 @@
     <t>WasteAnalysis</t>
   </si>
   <si>
-    <t>Get the FP diagrams for a plant state.</t>
-  </si>
-  <si>
-    <t>Get the exergy analysis for a plant state.</t>
-  </si>
-  <si>
-    <t>Import external data to a cTableData from CSV or XLSX files.</t>
-  </si>
-  <si>
-    <t>Display the list of the TaesLab result tables and their properties.</t>
-  </si>
-  <si>
-    <t>Get the productive diagrams of the plant.</t>
-  </si>
-  <si>
-    <t>Get the productive structure of the plant.</t>
-  </si>
-  <si>
     <t>Graphical user interface for displaying results interactively.</t>
   </si>
   <si>
-    <t>Save the result tables into a file.</t>
-  </si>
-  <si>
-    <t>Save the summary results into a file.</t>
-  </si>
-  <si>
-    <t>Display the graph associated with a results table.</t>
-  </si>
-  <si>
-    <t>Show the results tables in different formats.</t>
-  </si>
-  <si>
-    <t>Get the summary results for a plant.</t>
-  </si>
-  <si>
     <t>Graphical user interface for selecting thermoeconomic model parameters.</t>
   </si>
   <si>
     <t>Compatible user interface App for MATLAB/Octave.</t>
   </si>
   <si>
-    <t>Perform the termoeconomic analysis of a plant state.</t>
-  </si>
-  <si>
-    <t>Compare two states of the plant and make a thermoeconomic diagnosis</t>
-  </si>
-  <si>
     <t>MATLAB app for displaying results tables.</t>
   </si>
   <si>
-    <t>Waste recycling analysis of a plant state.</t>
-  </si>
-  <si>
     <t>buildMessage</t>
   </si>
   <si>
@@ -1281,33 +1239,9 @@
     <t>Implements the cReadModelStruct to read XML data model files.</t>
   </si>
   <si>
-    <t>Save the data model tables into a file.</t>
-  </si>
-  <si>
-    <t>Save the table into a file</t>
-  </si>
-  <si>
-    <t>Read a data model file.</t>
-  </si>
-  <si>
-    <t>Create a copy of a data model file in another format</t>
-  </si>
-  <si>
-    <t>Get a cDataModel object from a previously saved MAT file.</t>
-  </si>
-  <si>
-    <t>Exports the results tables into different formats.</t>
-  </si>
-  <si>
-    <t>Display, export, or save a table.</t>
-  </si>
-  <si>
     <t>Create a cThermoeconomicModel object from a data model.</t>
   </si>
   <si>
-    <t>Validate the table data model files.</t>
-  </si>
-  <si>
     <t>Plot the Waste Allocation graph.</t>
   </si>
   <si>
@@ -1420,6 +1354,72 @@
   </si>
   <si>
     <t>Identifies if the function has been executed in Octave.</t>
+  </si>
+  <si>
+    <t>Copy and convert a data model file to a different format.</t>
+  </si>
+  <si>
+    <t>Generate annotated fuel-product diagrams with exergy flows and costs.</t>
+  </si>
+  <si>
+    <t>Perform exergy analysis for a specific plant operating state.</t>
+  </si>
+  <si>
+    <t>Export result tables to various MATLAB data formats.</t>
+  </si>
+  <si>
+    <t>Import external tabular data from CSV or Excel files.</t>
+  </si>
+  <si>
+    <t>Load a cDataModel object from a MAT file.</t>
+  </si>
+  <si>
+    <t>Display catalog of available result tables and their properties.</t>
+  </si>
+  <si>
+    <t>Generate graph adjacency tables for productive structure visualization.</t>
+  </si>
+  <si>
+    <t>Extract and display productive structure information from a data model.</t>
+  </si>
+  <si>
+    <t>Read and validate a thermoeconomic data model file.</t>
+  </si>
+  <si>
+    <t>Save thermoeconomic data model to file in various formats.</t>
+  </si>
+  <si>
+    <t>Export result tables to file in multiple formats.</t>
+  </si>
+  <si>
+    <t>Export summary comparison tables for multiple states or cost samples.</t>
+  </si>
+  <si>
+    <t>Export a single table to file in various formats.</t>
+  </si>
+  <si>
+    <t>Display graphical visualizations of thermoeconomic analysis results.</t>
+  </si>
+  <si>
+    <t>Display and save result tables from thermoeconomic analyses.</t>
+  </si>
+  <si>
+    <t>Display, export, and save individual result tables.</t>
+  </si>
+  <si>
+    <t>Generate comparative summary tables across multiple operating conditions.</t>
+  </si>
+  <si>
+    <t>Perform thermoeconomic cost analysis of a plant operating state.</t>
+  </si>
+  <si>
+    <t>Detect and quantify malfunctions by comparing plant operating states.</t>
+  </si>
+  <si>
+    <t>Validate and convert tabular data model files.</t>
+  </si>
+  <si>
+    <t>Analyze waste cost allocation and recycling optimization strategies.</t>
   </si>
 </sst>
 </file>
@@ -1457,7 +1457,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="21">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -1587,90 +1587,6 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="hair">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="hair">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="hair">
-        <color indexed="64"/>
-      </left>
-      <right style="hair">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="hair">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="hair">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="hair">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="hair">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="hair">
-        <color indexed="64"/>
-      </left>
-      <right style="hair">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="hair">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -1742,6 +1658,51 @@
         <color indexed="64"/>
       </right>
       <top/>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="hair">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color indexed="64"/>
+      </left>
+      <right style="hair">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom style="hair">
         <color indexed="64"/>
       </bottom>
@@ -1751,7 +1712,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1764,17 +1725,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2128,66 +2086,66 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>394</v>
+        <v>380</v>
       </c>
       <c r="D1" t="s">
-        <v>395</v>
+        <v>381</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>195</v>
+        <v>181</v>
       </c>
       <c r="B2" t="s">
-        <v>405</v>
+        <v>391</v>
       </c>
       <c r="C2" t="s">
-        <v>397</v>
+        <v>383</v>
       </c>
       <c r="D2" t="s">
-        <v>401</v>
+        <v>387</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>196</v>
+        <v>182</v>
       </c>
       <c r="B3" t="s">
-        <v>406</v>
+        <v>392</v>
       </c>
       <c r="C3" t="s">
-        <v>398</v>
+        <v>384</v>
       </c>
       <c r="D3" t="s">
-        <v>402</v>
+        <v>388</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>197</v>
+        <v>183</v>
       </c>
       <c r="B4" t="s">
-        <v>407</v>
+        <v>393</v>
       </c>
       <c r="C4" t="s">
-        <v>399</v>
+        <v>385</v>
       </c>
       <c r="D4" t="s">
-        <v>403</v>
+        <v>389</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>396</v>
+        <v>382</v>
       </c>
       <c r="B5" t="s">
-        <v>408</v>
+        <v>394</v>
       </c>
       <c r="C5" t="s">
-        <v>400</v>
+        <v>386</v>
       </c>
       <c r="D5" t="s">
-        <v>404</v>
+        <v>390</v>
       </c>
     </row>
   </sheetData>
@@ -2199,8 +2157,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2211,46 +2169,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="14" t="s">
-        <v>214</v>
+      <c r="C1" s="2" t="s">
+        <v>200</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>424</v>
-      </c>
-      <c r="C2" s="5">
+      <c r="A2" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>450</v>
+      </c>
+      <c r="C2" s="19">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>418</v>
+        <v>461</v>
       </c>
       <c r="C3" s="5">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="10" t="s">
-        <v>419</v>
-      </c>
-      <c r="C4" s="11">
+      <c r="B4" s="3" t="s">
+        <v>441</v>
+      </c>
+      <c r="C4" s="5">
         <v>1</v>
       </c>
     </row>
@@ -2259,7 +2217,7 @@
         <v>7</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>420</v>
+        <v>446</v>
       </c>
       <c r="C5" s="5">
         <v>1</v>
@@ -2270,7 +2228,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>31</v>
+        <v>445</v>
       </c>
       <c r="C6" s="5">
         <v>1</v>
@@ -2281,7 +2239,7 @@
         <v>25</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>423</v>
+        <v>402</v>
       </c>
       <c r="C7" s="5">
         <v>2</v>
@@ -2292,7 +2250,7 @@
         <v>10</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>34</v>
+        <v>449</v>
       </c>
       <c r="C8" s="5">
         <v>2</v>
@@ -2303,7 +2261,7 @@
         <v>9</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>33</v>
+        <v>448</v>
       </c>
       <c r="C9" s="5">
         <v>2</v>
@@ -2314,7 +2272,7 @@
         <v>4</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>30</v>
+        <v>443</v>
       </c>
       <c r="C10" s="5">
         <v>2</v>
@@ -2325,7 +2283,7 @@
         <v>23</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>43</v>
+        <v>459</v>
       </c>
       <c r="C11" s="5">
         <v>2</v>
@@ -2336,7 +2294,7 @@
         <v>24</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>44</v>
+        <v>460</v>
       </c>
       <c r="C12" s="5">
         <v>2</v>
@@ -2347,7 +2305,7 @@
         <v>3</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>29</v>
+        <v>442</v>
       </c>
       <c r="C13" s="5">
         <v>2</v>
@@ -2358,7 +2316,7 @@
         <v>28</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>46</v>
+        <v>462</v>
       </c>
       <c r="C14" s="5">
         <v>2</v>
@@ -2369,7 +2327,7 @@
         <v>20</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>40</v>
+        <v>458</v>
       </c>
       <c r="C15" s="5">
         <v>2</v>
@@ -2377,10 +2335,10 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>36</v>
+        <v>451</v>
       </c>
       <c r="C16" s="5">
         <v>3</v>
@@ -2388,10 +2346,10 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>416</v>
+        <v>452</v>
       </c>
       <c r="C17" s="5">
         <v>3</v>
@@ -2402,7 +2360,7 @@
         <v>15</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>37</v>
+        <v>453</v>
       </c>
       <c r="C18" s="5">
         <v>3</v>
@@ -2413,7 +2371,7 @@
         <v>16</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>417</v>
+        <v>454</v>
       </c>
       <c r="C19" s="5">
         <v>3</v>
@@ -2424,7 +2382,7 @@
         <v>8</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>32</v>
+        <v>447</v>
       </c>
       <c r="C20" s="5">
         <v>4</v>
@@ -2432,10 +2390,10 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>39</v>
+        <v>455</v>
       </c>
       <c r="C21" s="5">
         <v>4</v>
@@ -2443,10 +2401,10 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>422</v>
+        <v>456</v>
       </c>
       <c r="C22" s="5">
         <v>4</v>
@@ -2454,10 +2412,10 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>38</v>
+        <v>457</v>
       </c>
       <c r="C23" s="5">
         <v>4</v>
@@ -2468,7 +2426,7 @@
         <v>5</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>421</v>
+        <v>444</v>
       </c>
       <c r="C24" s="5">
         <v>4</v>
@@ -2479,7 +2437,7 @@
         <v>22</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="C25" s="5">
         <v>5</v>
@@ -2490,7 +2448,7 @@
         <v>21</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="C26" s="5">
         <v>5</v>
@@ -2501,7 +2459,7 @@
         <v>12</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="C27" s="5">
         <v>5</v>
@@ -2512,7 +2470,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="C28" s="8">
         <v>5</v>
@@ -2531,8 +2489,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2553,358 +2511,358 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>214</v>
+        <v>200</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>415</v>
+      </c>
+      <c r="C2" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
+        <v>412</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>416</v>
+      </c>
+      <c r="C3" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>417</v>
+      </c>
+      <c r="C4" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>418</v>
+      </c>
+      <c r="C5" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
+        <v>413</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>419</v>
+      </c>
+      <c r="C6" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>420</v>
+      </c>
+      <c r="C7" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>421</v>
+      </c>
+      <c r="C8" s="11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>414</v>
+      </c>
+      <c r="C9" s="11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="C10" s="11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B11" s="16" t="s">
+        <v>439</v>
+      </c>
+      <c r="C11" s="11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="B12" s="16" t="s">
+        <v>440</v>
+      </c>
+      <c r="C12" s="11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B13" s="9" t="s">
+        <v>422</v>
+      </c>
+      <c r="C13" s="11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="C14" s="11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>423</v>
+      </c>
+      <c r="C15" s="11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="C16" s="11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="C17" s="11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>424</v>
+      </c>
+      <c r="C18" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>425</v>
+      </c>
+      <c r="C19" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>426</v>
+      </c>
+      <c r="C20" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>427</v>
+      </c>
+      <c r="C21" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>428</v>
+      </c>
+      <c r="C22" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>429</v>
+      </c>
+      <c r="C23" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>430</v>
+      </c>
+      <c r="C24" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>431</v>
+      </c>
+      <c r="C25" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="B26" s="9" t="s">
+        <v>432</v>
+      </c>
+      <c r="C26" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>433</v>
+      </c>
+      <c r="C27" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="B28" s="9" t="s">
+        <v>434</v>
+      </c>
+      <c r="C28" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="B29" s="9" t="s">
+        <v>435</v>
+      </c>
+      <c r="C29" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="B30" s="9" t="s">
+        <v>436</v>
+      </c>
+      <c r="C30" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="B31" s="9" t="s">
         <v>437</v>
       </c>
-      <c r="C2" s="20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="15" t="s">
-        <v>434</v>
-      </c>
-      <c r="B3" s="15" t="s">
+      <c r="C31" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B32" s="9" t="s">
         <v>438</v>
       </c>
-      <c r="C3" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="B4" s="15" t="s">
-        <v>439</v>
-      </c>
-      <c r="C4" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="B5" s="15" t="s">
-        <v>440</v>
-      </c>
-      <c r="C5" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="15" t="s">
-        <v>435</v>
-      </c>
-      <c r="B6" s="15" t="s">
-        <v>441</v>
-      </c>
-      <c r="C6" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="B7" s="15" t="s">
-        <v>442</v>
-      </c>
-      <c r="C7" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="15" t="s">
-        <v>56</v>
-      </c>
-      <c r="B8" s="15" t="s">
-        <v>443</v>
-      </c>
-      <c r="C8" s="17">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="B9" s="15" t="s">
-        <v>436</v>
-      </c>
-      <c r="C9" s="17">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="B10" s="15" t="s">
-        <v>78</v>
-      </c>
-      <c r="C10" s="17">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="B11" s="22" t="s">
-        <v>461</v>
-      </c>
-      <c r="C11" s="17">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="15" t="s">
+      <c r="C32" s="11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="B33" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="B12" s="22" t="s">
-        <v>462</v>
-      </c>
-      <c r="C12" s="17">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="15" t="s">
-        <v>64</v>
-      </c>
-      <c r="B13" s="15" t="s">
-        <v>444</v>
-      </c>
-      <c r="C13" s="17">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="B14" s="15" t="s">
-        <v>79</v>
-      </c>
-      <c r="C14" s="17">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="B15" s="15" t="s">
-        <v>445</v>
-      </c>
-      <c r="C15" s="17">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="B16" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="C16" s="17">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="15" t="s">
-        <v>65</v>
-      </c>
-      <c r="B17" s="15" t="s">
-        <v>81</v>
-      </c>
-      <c r="C17" s="17">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="15" t="s">
-        <v>75</v>
-      </c>
-      <c r="B18" s="15" t="s">
-        <v>446</v>
-      </c>
-      <c r="C18" s="17">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="B19" s="15" t="s">
-        <v>447</v>
-      </c>
-      <c r="C19" s="17">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="B20" s="15" t="s">
-        <v>448</v>
-      </c>
-      <c r="C20" s="17">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="15" t="s">
-        <v>67</v>
-      </c>
-      <c r="B21" s="15" t="s">
-        <v>449</v>
-      </c>
-      <c r="C21" s="17">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="15" t="s">
-        <v>68</v>
-      </c>
-      <c r="B22" s="15" t="s">
-        <v>450</v>
-      </c>
-      <c r="C22" s="17">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="15" t="s">
-        <v>73</v>
-      </c>
-      <c r="B23" s="15" t="s">
-        <v>451</v>
-      </c>
-      <c r="C23" s="17">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="15" t="s">
-        <v>76</v>
-      </c>
-      <c r="B24" s="15" t="s">
-        <v>452</v>
-      </c>
-      <c r="C24" s="17">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="B25" s="15" t="s">
-        <v>453</v>
-      </c>
-      <c r="C25" s="17">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="15" t="s">
-        <v>66</v>
-      </c>
-      <c r="B26" s="15" t="s">
-        <v>454</v>
-      </c>
-      <c r="C26" s="17">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="15" t="s">
-        <v>69</v>
-      </c>
-      <c r="B27" s="15" t="s">
-        <v>455</v>
-      </c>
-      <c r="C27" s="17">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="B28" s="15" t="s">
-        <v>456</v>
-      </c>
-      <c r="C28" s="17">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="15" t="s">
-        <v>71</v>
-      </c>
-      <c r="B29" s="15" t="s">
-        <v>457</v>
-      </c>
-      <c r="C29" s="17">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="15" t="s">
-        <v>72</v>
-      </c>
-      <c r="B30" s="15" t="s">
-        <v>458</v>
-      </c>
-      <c r="C30" s="17">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="15" t="s">
-        <v>74</v>
-      </c>
-      <c r="B31" s="15" t="s">
-        <v>459</v>
-      </c>
-      <c r="C31" s="17">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="B32" s="15" t="s">
-        <v>460</v>
-      </c>
-      <c r="C32" s="17">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="B33" s="16" t="s">
-        <v>77</v>
-      </c>
-      <c r="C33" s="18">
+      <c r="C33" s="12">
         <v>4</v>
       </c>
     </row>
@@ -2940,677 +2898,677 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>214</v>
+        <v>200</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>175</v>
+      </c>
+      <c r="C2" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="C3" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="C4" s="11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="C5" s="11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="C6" s="11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>156</v>
+      </c>
+      <c r="C7" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="C8" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="C9" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>401</v>
+      </c>
+      <c r="C10" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="C11" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>157</v>
+      </c>
+      <c r="C12" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>400</v>
+      </c>
+      <c r="C13" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="C14" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="C15" s="11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="C16" s="11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="C17" s="11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="C18" s="11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>409</v>
+      </c>
+      <c r="C19" s="11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="C20" s="11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="C21" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="C22" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="C23" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="C24" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="C25" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="B26" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="C26" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="C27" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="B28" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="C28" s="11">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="B29" s="9" t="s">
         <v>137</v>
       </c>
-      <c r="B2" s="15" t="s">
-        <v>189</v>
-      </c>
-      <c r="C2" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="19" t="s">
-        <v>105</v>
-      </c>
-      <c r="B3" s="19" t="s">
-        <v>161</v>
-      </c>
-      <c r="C3" s="20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="15" t="s">
-        <v>139</v>
-      </c>
-      <c r="B4" s="15" t="s">
-        <v>191</v>
-      </c>
-      <c r="C4" s="17">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="15" t="s">
-        <v>106</v>
-      </c>
-      <c r="B5" s="15" t="s">
-        <v>162</v>
-      </c>
-      <c r="C5" s="17">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="15" t="s">
-        <v>110</v>
-      </c>
-      <c r="B6" s="15" t="s">
+      <c r="C29" s="11">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="B30" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="C30" s="11">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="B31" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="C31" s="11">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="B32" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="C32" s="11">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="B33" s="9" t="s">
         <v>166</v>
       </c>
-      <c r="C6" s="17">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="15" t="s">
-        <v>114</v>
-      </c>
-      <c r="B7" s="15" t="s">
+      <c r="C33" s="11">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="B34" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="C34" s="11">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="B35" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="C35" s="11">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="B36" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="C36" s="11">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="B37" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="C37" s="11">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="B38" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="C38" s="11">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="B39" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="C39" s="11">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="B40" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="C40" s="11">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="B41" s="9" t="s">
+        <v>174</v>
+      </c>
+      <c r="C41" s="11">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="B42" s="9" t="s">
         <v>170</v>
       </c>
-      <c r="C7" s="17">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="15" t="s">
-        <v>117</v>
-      </c>
-      <c r="B8" s="15" t="s">
+      <c r="C42" s="11">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="B43" s="9" t="s">
         <v>173</v>
       </c>
-      <c r="C8" s="17">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="15" t="s">
-        <v>116</v>
-      </c>
-      <c r="B9" s="15" t="s">
-        <v>172</v>
-      </c>
-      <c r="C9" s="17">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="15" t="s">
-        <v>120</v>
-      </c>
-      <c r="B10" s="15" t="s">
-        <v>415</v>
-      </c>
-      <c r="C10" s="17">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="15" t="s">
-        <v>118</v>
-      </c>
-      <c r="B11" s="15" t="s">
-        <v>174</v>
-      </c>
-      <c r="C11" s="17">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="15" t="s">
-        <v>115</v>
-      </c>
-      <c r="B12" s="15" t="s">
-        <v>171</v>
-      </c>
-      <c r="C12" s="17">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="15" t="s">
-        <v>119</v>
-      </c>
-      <c r="B13" s="15" t="s">
-        <v>414</v>
-      </c>
-      <c r="C13" s="17">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="15" t="s">
-        <v>109</v>
-      </c>
-      <c r="B14" s="15" t="s">
+      <c r="C43" s="11">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="B44" s="9" t="s">
+        <v>406</v>
+      </c>
+      <c r="C44" s="11">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="B45" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="C45" s="11">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="B46" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="C46" s="11">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="B47" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="C47" s="11">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="B48" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="C48" s="11">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="B49" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="C49" s="11">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="B50" s="9" t="s">
+        <v>403</v>
+      </c>
+      <c r="C50" s="11">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="B51" s="9" t="s">
+        <v>404</v>
+      </c>
+      <c r="C51" s="11">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="B52" s="9" t="s">
+        <v>405</v>
+      </c>
+      <c r="C52" s="11">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="B53" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="C53" s="11">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="B54" s="9" t="s">
+        <v>407</v>
+      </c>
+      <c r="C54" s="11">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="B55" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="C55" s="11">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="B56" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="C56" s="11">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="B57" s="9" t="s">
+        <v>178</v>
+      </c>
+      <c r="C57" s="11">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="B58" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="C58" s="11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="B59" s="9" t="s">
+        <v>408</v>
+      </c>
+      <c r="C59" s="11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="B60" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="C60" s="11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="B61" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="C61" s="11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="B62" s="10" t="s">
         <v>165</v>
       </c>
-      <c r="C14" s="17">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="15" t="s">
-        <v>112</v>
-      </c>
-      <c r="B15" s="15" t="s">
-        <v>168</v>
-      </c>
-      <c r="C15" s="17">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="15" t="s">
-        <v>93</v>
-      </c>
-      <c r="B16" s="15" t="s">
-        <v>152</v>
-      </c>
-      <c r="C16" s="17">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="15" t="s">
-        <v>95</v>
-      </c>
-      <c r="B17" s="15" t="s">
-        <v>154</v>
-      </c>
-      <c r="C17" s="17">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="15" t="s">
-        <v>125</v>
-      </c>
-      <c r="B18" s="15" t="s">
-        <v>178</v>
-      </c>
-      <c r="C18" s="17">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="15" t="s">
-        <v>121</v>
-      </c>
-      <c r="B19" s="15" t="s">
-        <v>431</v>
-      </c>
-      <c r="C19" s="17">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="15" t="s">
-        <v>142</v>
-      </c>
-      <c r="B20" s="15" t="s">
-        <v>194</v>
-      </c>
-      <c r="C20" s="17">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="15" t="s">
-        <v>122</v>
-      </c>
-      <c r="B21" s="15" t="s">
-        <v>175</v>
-      </c>
-      <c r="C21" s="17">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="15" t="s">
-        <v>124</v>
-      </c>
-      <c r="B22" s="15" t="s">
-        <v>177</v>
-      </c>
-      <c r="C22" s="17">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="15" t="s">
-        <v>85</v>
-      </c>
-      <c r="B23" s="15" t="s">
-        <v>145</v>
-      </c>
-      <c r="C23" s="17">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="15" t="s">
-        <v>138</v>
-      </c>
-      <c r="B24" s="15" t="s">
-        <v>190</v>
-      </c>
-      <c r="C24" s="17">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="15" t="s">
-        <v>123</v>
-      </c>
-      <c r="B25" s="15" t="s">
-        <v>176</v>
-      </c>
-      <c r="C25" s="17">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="15" t="s">
-        <v>107</v>
-      </c>
-      <c r="B26" s="15" t="s">
-        <v>163</v>
-      </c>
-      <c r="C26" s="17">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="15" t="s">
-        <v>108</v>
-      </c>
-      <c r="B27" s="15" t="s">
-        <v>164</v>
-      </c>
-      <c r="C27" s="17">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="B28" s="15" t="s">
-        <v>153</v>
-      </c>
-      <c r="C28" s="17">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="15" t="s">
-        <v>92</v>
-      </c>
-      <c r="B29" s="15" t="s">
-        <v>151</v>
-      </c>
-      <c r="C29" s="17">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="15" t="s">
-        <v>87</v>
-      </c>
-      <c r="B30" s="15" t="s">
-        <v>147</v>
-      </c>
-      <c r="C30" s="17">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="15" t="s">
-        <v>141</v>
-      </c>
-      <c r="B31" s="15" t="s">
-        <v>193</v>
-      </c>
-      <c r="C31" s="17">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="15" t="s">
-        <v>128</v>
-      </c>
-      <c r="B32" s="15" t="s">
-        <v>181</v>
-      </c>
-      <c r="C32" s="17">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="15" t="s">
-        <v>127</v>
-      </c>
-      <c r="B33" s="15" t="s">
-        <v>180</v>
-      </c>
-      <c r="C33" s="17">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="15" t="s">
-        <v>129</v>
-      </c>
-      <c r="B34" s="15" t="s">
-        <v>182</v>
-      </c>
-      <c r="C34" s="17">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="15" t="s">
-        <v>91</v>
-      </c>
-      <c r="B35" s="15" t="s">
-        <v>150</v>
-      </c>
-      <c r="C35" s="17">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="15" t="s">
-        <v>88</v>
-      </c>
-      <c r="B36" s="15" t="s">
-        <v>148</v>
-      </c>
-      <c r="C36" s="17">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="15" t="s">
-        <v>111</v>
-      </c>
-      <c r="B37" s="15" t="s">
-        <v>167</v>
-      </c>
-      <c r="C37" s="17">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="15" t="s">
-        <v>130</v>
-      </c>
-      <c r="B38" s="15" t="s">
-        <v>183</v>
-      </c>
-      <c r="C38" s="17">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="15" t="s">
-        <v>133</v>
-      </c>
-      <c r="B39" s="15" t="s">
-        <v>186</v>
-      </c>
-      <c r="C39" s="17">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="15" t="s">
-        <v>132</v>
-      </c>
-      <c r="B40" s="15" t="s">
-        <v>185</v>
-      </c>
-      <c r="C40" s="17">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="15" t="s">
-        <v>135</v>
-      </c>
-      <c r="B41" s="15" t="s">
-        <v>188</v>
-      </c>
-      <c r="C41" s="17">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="15" t="s">
-        <v>131</v>
-      </c>
-      <c r="B42" s="15" t="s">
-        <v>184</v>
-      </c>
-      <c r="C42" s="17">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="15" t="s">
-        <v>134</v>
-      </c>
-      <c r="B43" s="15" t="s">
-        <v>187</v>
-      </c>
-      <c r="C43" s="17">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="15" t="s">
-        <v>136</v>
-      </c>
-      <c r="B44" s="15" t="s">
-        <v>428</v>
-      </c>
-      <c r="C44" s="17">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="15" t="s">
-        <v>101</v>
-      </c>
-      <c r="B45" s="15" t="s">
-        <v>159</v>
-      </c>
-      <c r="C45" s="17">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="15" t="s">
-        <v>96</v>
-      </c>
-      <c r="B46" s="15" t="s">
-        <v>155</v>
-      </c>
-      <c r="C46" s="17">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="15" t="s">
-        <v>97</v>
-      </c>
-      <c r="B47" s="15" t="s">
-        <v>156</v>
-      </c>
-      <c r="C47" s="17">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="15" t="s">
-        <v>98</v>
-      </c>
-      <c r="B48" s="15" t="s">
-        <v>157</v>
-      </c>
-      <c r="C48" s="17">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="15" t="s">
-        <v>99</v>
-      </c>
-      <c r="B49" s="15" t="s">
-        <v>158</v>
-      </c>
-      <c r="C49" s="17">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="15" t="s">
-        <v>103</v>
-      </c>
-      <c r="B50" s="15" t="s">
-        <v>425</v>
-      </c>
-      <c r="C50" s="17">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" s="15" t="s">
-        <v>100</v>
-      </c>
-      <c r="B51" s="15" t="s">
-        <v>426</v>
-      </c>
-      <c r="C51" s="17">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" s="15" t="s">
-        <v>102</v>
-      </c>
-      <c r="B52" s="15" t="s">
-        <v>427</v>
-      </c>
-      <c r="C52" s="17">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" s="15" t="s">
-        <v>90</v>
-      </c>
-      <c r="B53" s="15" t="s">
-        <v>149</v>
-      </c>
-      <c r="C53" s="17">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="B54" s="15" t="s">
-        <v>429</v>
-      </c>
-      <c r="C54" s="17">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" s="15" t="s">
-        <v>83</v>
-      </c>
-      <c r="B55" s="15" t="s">
-        <v>143</v>
-      </c>
-      <c r="C55" s="17">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" s="15" t="s">
-        <v>84</v>
-      </c>
-      <c r="B56" s="15" t="s">
-        <v>144</v>
-      </c>
-      <c r="C56" s="17">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57" s="15" t="s">
-        <v>140</v>
-      </c>
-      <c r="B57" s="15" t="s">
-        <v>192</v>
-      </c>
-      <c r="C57" s="17">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58" s="15" t="s">
-        <v>104</v>
-      </c>
-      <c r="B58" s="15" t="s">
-        <v>160</v>
-      </c>
-      <c r="C58" s="17">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59" s="15" t="s">
-        <v>89</v>
-      </c>
-      <c r="B59" s="15" t="s">
-        <v>430</v>
-      </c>
-      <c r="C59" s="17">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60" s="15" t="s">
-        <v>86</v>
-      </c>
-      <c r="B60" s="15" t="s">
-        <v>146</v>
-      </c>
-      <c r="C60" s="17">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61" s="15" t="s">
-        <v>113</v>
-      </c>
-      <c r="B61" s="15" t="s">
-        <v>169</v>
-      </c>
-      <c r="C61" s="17">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62" s="16" t="s">
-        <v>126</v>
-      </c>
-      <c r="B62" s="16" t="s">
-        <v>179</v>
-      </c>
-      <c r="C62" s="18">
+      <c r="C62" s="12">
         <v>10</v>
       </c>
     </row>
@@ -3646,15 +3604,15 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>214</v>
+        <v>200</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>215</v>
+        <v>201</v>
       </c>
       <c r="B2" t="s">
-        <v>216</v>
+        <v>202</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -3662,10 +3620,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>217</v>
+        <v>203</v>
       </c>
       <c r="B3" t="s">
-        <v>218</v>
+        <v>204</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -3673,10 +3631,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>219</v>
+        <v>205</v>
       </c>
       <c r="B4" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -3684,10 +3642,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>221</v>
+        <v>207</v>
       </c>
       <c r="B5" t="s">
-        <v>222</v>
+        <v>208</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -3695,10 +3653,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>223</v>
+        <v>209</v>
       </c>
       <c r="B6" t="s">
-        <v>224</v>
+        <v>210</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -3706,10 +3664,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>225</v>
+        <v>211</v>
       </c>
       <c r="B7" t="s">
-        <v>226</v>
+        <v>212</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -3717,10 +3675,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>227</v>
+        <v>213</v>
       </c>
       <c r="B8" t="s">
-        <v>409</v>
+        <v>395</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -3728,10 +3686,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>228</v>
+        <v>214</v>
       </c>
       <c r="B9" t="s">
-        <v>229</v>
+        <v>215</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -3739,10 +3697,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>230</v>
+        <v>216</v>
       </c>
       <c r="B10" t="s">
-        <v>231</v>
+        <v>217</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -3750,10 +3708,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>232</v>
+        <v>218</v>
       </c>
       <c r="B11" t="s">
-        <v>233</v>
+        <v>219</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -3761,10 +3719,10 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>234</v>
+        <v>220</v>
       </c>
       <c r="B12" t="s">
-        <v>235</v>
+        <v>221</v>
       </c>
       <c r="C12">
         <v>2</v>
@@ -3772,10 +3730,10 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>236</v>
+        <v>222</v>
       </c>
       <c r="B13" t="s">
-        <v>237</v>
+        <v>223</v>
       </c>
       <c r="C13">
         <v>2</v>
@@ -3783,10 +3741,10 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>238</v>
+        <v>224</v>
       </c>
       <c r="B14" t="s">
-        <v>239</v>
+        <v>225</v>
       </c>
       <c r="C14">
         <v>2</v>
@@ -3794,10 +3752,10 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>240</v>
+        <v>226</v>
       </c>
       <c r="B15" t="s">
-        <v>241</v>
+        <v>227</v>
       </c>
       <c r="C15">
         <v>2</v>
@@ -3805,10 +3763,10 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>242</v>
+        <v>228</v>
       </c>
       <c r="B16" t="s">
-        <v>243</v>
+        <v>229</v>
       </c>
       <c r="C16">
         <v>2</v>
@@ -3816,10 +3774,10 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>244</v>
+        <v>230</v>
       </c>
       <c r="B17" t="s">
-        <v>245</v>
+        <v>231</v>
       </c>
       <c r="C17">
         <v>2</v>
@@ -3827,10 +3785,10 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>246</v>
+        <v>232</v>
       </c>
       <c r="B18" t="s">
-        <v>247</v>
+        <v>233</v>
       </c>
       <c r="C18">
         <v>2</v>
@@ -3838,10 +3796,10 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>248</v>
+        <v>234</v>
       </c>
       <c r="B19" t="s">
-        <v>249</v>
+        <v>235</v>
       </c>
       <c r="C19">
         <v>2</v>
@@ -3849,10 +3807,10 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>250</v>
+        <v>236</v>
       </c>
       <c r="B20" t="s">
-        <v>251</v>
+        <v>237</v>
       </c>
       <c r="C20">
         <v>2</v>
@@ -3860,10 +3818,10 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>252</v>
+        <v>238</v>
       </c>
       <c r="B21" t="s">
-        <v>253</v>
+        <v>239</v>
       </c>
       <c r="C21">
         <v>2</v>
@@ -3871,10 +3829,10 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>254</v>
+        <v>240</v>
       </c>
       <c r="B22" t="s">
-        <v>255</v>
+        <v>241</v>
       </c>
       <c r="C22">
         <v>2</v>
@@ -3882,10 +3840,10 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>256</v>
+        <v>242</v>
       </c>
       <c r="B23" t="s">
-        <v>257</v>
+        <v>243</v>
       </c>
       <c r="C23">
         <v>3</v>
@@ -3893,10 +3851,10 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>258</v>
+        <v>244</v>
       </c>
       <c r="B24" t="s">
-        <v>259</v>
+        <v>245</v>
       </c>
       <c r="C24">
         <v>3</v>
@@ -3904,10 +3862,10 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>260</v>
+        <v>246</v>
       </c>
       <c r="B25" t="s">
-        <v>261</v>
+        <v>247</v>
       </c>
       <c r="C25">
         <v>3</v>
@@ -3915,10 +3873,10 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>262</v>
+        <v>248</v>
       </c>
       <c r="B26" t="s">
-        <v>410</v>
+        <v>396</v>
       </c>
       <c r="C26">
         <v>3</v>
@@ -3926,10 +3884,10 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>263</v>
+        <v>249</v>
       </c>
       <c r="B27" t="s">
-        <v>264</v>
+        <v>250</v>
       </c>
       <c r="C27">
         <v>3</v>
@@ -3937,10 +3895,10 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>265</v>
+        <v>251</v>
       </c>
       <c r="B28" t="s">
-        <v>266</v>
+        <v>252</v>
       </c>
       <c r="C28">
         <v>3</v>
@@ -3948,10 +3906,10 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>267</v>
+        <v>253</v>
       </c>
       <c r="B29" t="s">
-        <v>268</v>
+        <v>254</v>
       </c>
       <c r="C29">
         <v>3</v>
@@ -3959,10 +3917,10 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
       <c r="B30" t="s">
-        <v>270</v>
+        <v>256</v>
       </c>
       <c r="C30">
         <v>4</v>
@@ -3970,10 +3928,10 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>271</v>
+        <v>257</v>
       </c>
       <c r="B31" t="s">
-        <v>272</v>
+        <v>258</v>
       </c>
       <c r="C31">
         <v>4</v>
@@ -3981,10 +3939,10 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>273</v>
+        <v>259</v>
       </c>
       <c r="B32" t="s">
-        <v>274</v>
+        <v>260</v>
       </c>
       <c r="C32">
         <v>4</v>
@@ -3992,10 +3950,10 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>275</v>
+        <v>261</v>
       </c>
       <c r="B33" t="s">
-        <v>276</v>
+        <v>262</v>
       </c>
       <c r="C33">
         <v>4</v>
@@ -4003,10 +3961,10 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>277</v>
+        <v>263</v>
       </c>
       <c r="B34" t="s">
-        <v>278</v>
+        <v>264</v>
       </c>
       <c r="C34">
         <v>4</v>
@@ -4014,10 +3972,10 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>279</v>
+        <v>265</v>
       </c>
       <c r="B35" t="s">
-        <v>280</v>
+        <v>266</v>
       </c>
       <c r="C35">
         <v>5</v>
@@ -4025,10 +3983,10 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>281</v>
+        <v>267</v>
       </c>
       <c r="B36" t="s">
-        <v>282</v>
+        <v>268</v>
       </c>
       <c r="C36">
         <v>5</v>
@@ -4036,10 +3994,10 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>283</v>
+        <v>269</v>
       </c>
       <c r="B37" t="s">
-        <v>284</v>
+        <v>270</v>
       </c>
       <c r="C37">
         <v>5</v>
@@ -4047,10 +4005,10 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>285</v>
+        <v>271</v>
       </c>
       <c r="B38" t="s">
-        <v>286</v>
+        <v>272</v>
       </c>
       <c r="C38">
         <v>5</v>
@@ -4058,10 +4016,10 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>287</v>
+        <v>273</v>
       </c>
       <c r="B39" t="s">
-        <v>288</v>
+        <v>274</v>
       </c>
       <c r="C39">
         <v>6</v>
@@ -4069,10 +4027,10 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>289</v>
+        <v>275</v>
       </c>
       <c r="B40" t="s">
-        <v>290</v>
+        <v>276</v>
       </c>
       <c r="C40">
         <v>6</v>
@@ -4080,10 +4038,10 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>291</v>
+        <v>277</v>
       </c>
       <c r="B41" t="s">
-        <v>292</v>
+        <v>278</v>
       </c>
       <c r="C41">
         <v>6</v>
@@ -4091,10 +4049,10 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>293</v>
+        <v>279</v>
       </c>
       <c r="B42" t="s">
-        <v>294</v>
+        <v>280</v>
       </c>
       <c r="C42">
         <v>6</v>
@@ -4102,10 +4060,10 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>295</v>
+        <v>281</v>
       </c>
       <c r="B43" t="s">
-        <v>296</v>
+        <v>282</v>
       </c>
       <c r="C43">
         <v>6</v>
@@ -4113,10 +4071,10 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>297</v>
+        <v>283</v>
       </c>
       <c r="B44" t="s">
-        <v>298</v>
+        <v>284</v>
       </c>
       <c r="C44">
         <v>6</v>
@@ -4124,10 +4082,10 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>299</v>
+        <v>285</v>
       </c>
       <c r="B45" t="s">
-        <v>411</v>
+        <v>397</v>
       </c>
       <c r="C45">
         <v>6</v>
@@ -4135,10 +4093,10 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>300</v>
+        <v>286</v>
       </c>
       <c r="B46" t="s">
-        <v>301</v>
+        <v>287</v>
       </c>
       <c r="C46">
         <v>6</v>
@@ -4146,10 +4104,10 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>302</v>
+        <v>288</v>
       </c>
       <c r="B47" t="s">
-        <v>303</v>
+        <v>289</v>
       </c>
       <c r="C47">
         <v>6</v>
@@ -4157,10 +4115,10 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>304</v>
+        <v>290</v>
       </c>
       <c r="B48" t="s">
-        <v>305</v>
+        <v>291</v>
       </c>
       <c r="C48">
         <v>6</v>
@@ -4168,10 +4126,10 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>306</v>
+        <v>292</v>
       </c>
       <c r="B49" t="s">
-        <v>307</v>
+        <v>293</v>
       </c>
       <c r="C49">
         <v>6</v>
@@ -4179,10 +4137,10 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>308</v>
+        <v>294</v>
       </c>
       <c r="B50" t="s">
-        <v>309</v>
+        <v>295</v>
       </c>
       <c r="C50">
         <v>6</v>
@@ -4190,10 +4148,10 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>310</v>
+        <v>296</v>
       </c>
       <c r="B51" t="s">
-        <v>311</v>
+        <v>297</v>
       </c>
       <c r="C51">
         <v>6</v>
@@ -4201,10 +4159,10 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>312</v>
+        <v>298</v>
       </c>
       <c r="B52" t="s">
-        <v>313</v>
+        <v>299</v>
       </c>
       <c r="C52">
         <v>6</v>
@@ -4212,10 +4170,10 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>314</v>
+        <v>300</v>
       </c>
       <c r="B53" t="s">
-        <v>315</v>
+        <v>301</v>
       </c>
       <c r="C53">
         <v>6</v>
@@ -4223,10 +4181,10 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>316</v>
+        <v>302</v>
       </c>
       <c r="B54" t="s">
-        <v>317</v>
+        <v>303</v>
       </c>
       <c r="C54">
         <v>6</v>
@@ -4234,10 +4192,10 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>318</v>
+        <v>304</v>
       </c>
       <c r="B55" t="s">
-        <v>319</v>
+        <v>305</v>
       </c>
       <c r="C55">
         <v>6</v>
@@ -4245,10 +4203,10 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>320</v>
+        <v>306</v>
       </c>
       <c r="B56" t="s">
-        <v>321</v>
+        <v>307</v>
       </c>
       <c r="C56">
         <v>6</v>
@@ -4256,10 +4214,10 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>322</v>
+        <v>308</v>
       </c>
       <c r="B57" t="s">
-        <v>323</v>
+        <v>309</v>
       </c>
       <c r="C57">
         <v>7</v>
@@ -4267,10 +4225,10 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>324</v>
+        <v>310</v>
       </c>
       <c r="B58" t="s">
-        <v>325</v>
+        <v>311</v>
       </c>
       <c r="C58">
         <v>7</v>
@@ -4278,10 +4236,10 @@
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>326</v>
+        <v>312</v>
       </c>
       <c r="B59" t="s">
-        <v>327</v>
+        <v>313</v>
       </c>
       <c r="C59">
         <v>7</v>
@@ -4289,10 +4247,10 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>328</v>
+        <v>314</v>
       </c>
       <c r="B60" t="s">
-        <v>329</v>
+        <v>315</v>
       </c>
       <c r="C60">
         <v>7</v>
@@ -4300,10 +4258,10 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>330</v>
+        <v>316</v>
       </c>
       <c r="B61" t="s">
-        <v>331</v>
+        <v>317</v>
       </c>
       <c r="C61">
         <v>8</v>
@@ -4311,10 +4269,10 @@
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>332</v>
+        <v>318</v>
       </c>
       <c r="B62" t="s">
-        <v>333</v>
+        <v>319</v>
       </c>
       <c r="C62">
         <v>8</v>
@@ -4322,10 +4280,10 @@
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>334</v>
+        <v>320</v>
       </c>
       <c r="B63" t="s">
-        <v>412</v>
+        <v>398</v>
       </c>
       <c r="C63">
         <v>8</v>
@@ -4333,10 +4291,10 @@
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>335</v>
+        <v>321</v>
       </c>
       <c r="B64" t="s">
-        <v>336</v>
+        <v>322</v>
       </c>
       <c r="C64">
         <v>8</v>
@@ -4344,10 +4302,10 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>337</v>
+        <v>323</v>
       </c>
       <c r="B65" t="s">
-        <v>338</v>
+        <v>324</v>
       </c>
       <c r="C65">
         <v>9</v>
@@ -4355,10 +4313,10 @@
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>339</v>
+        <v>325</v>
       </c>
       <c r="B66" t="s">
-        <v>340</v>
+        <v>326</v>
       </c>
       <c r="C66">
         <v>9</v>
@@ -4366,10 +4324,10 @@
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>341</v>
+        <v>327</v>
       </c>
       <c r="B67" t="s">
-        <v>338</v>
+        <v>324</v>
       </c>
       <c r="C67">
         <v>9</v>
@@ -4377,10 +4335,10 @@
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>342</v>
+        <v>328</v>
       </c>
       <c r="B68" t="s">
-        <v>413</v>
+        <v>399</v>
       </c>
       <c r="C68">
         <v>10</v>
@@ -4388,10 +4346,10 @@
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>343</v>
+        <v>329</v>
       </c>
       <c r="B69" t="s">
-        <v>344</v>
+        <v>330</v>
       </c>
       <c r="C69">
         <v>10</v>
@@ -4399,10 +4357,10 @@
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>345</v>
+        <v>331</v>
       </c>
       <c r="B70" t="s">
-        <v>346</v>
+        <v>332</v>
       </c>
       <c r="C70">
         <v>10</v>
@@ -4410,10 +4368,10 @@
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>347</v>
+        <v>333</v>
       </c>
       <c r="B71" t="s">
-        <v>348</v>
+        <v>334</v>
       </c>
       <c r="C71">
         <v>10</v>
@@ -4421,10 +4379,10 @@
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>349</v>
+        <v>335</v>
       </c>
       <c r="B72" t="s">
-        <v>350</v>
+        <v>336</v>
       </c>
       <c r="C72">
         <v>10</v>
@@ -4432,10 +4390,10 @@
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>351</v>
+        <v>337</v>
       </c>
       <c r="B73" t="s">
-        <v>352</v>
+        <v>338</v>
       </c>
       <c r="C73">
         <v>10</v>
@@ -4462,22 +4420,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="21" t="s">
-        <v>353</v>
+      <c r="C1" s="15" t="s">
+        <v>339</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>389</v>
+        <v>375</v>
       </c>
       <c r="B2" t="s">
-        <v>198</v>
+        <v>184</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -4485,10 +4443,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>390</v>
+        <v>376</v>
       </c>
       <c r="B3" t="s">
-        <v>199</v>
+        <v>185</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -4496,10 +4454,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>391</v>
+        <v>377</v>
       </c>
       <c r="B4" t="s">
-        <v>200</v>
+        <v>186</v>
       </c>
       <c r="C4">
         <v>3</v>
@@ -4507,10 +4465,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>392</v>
+        <v>378</v>
       </c>
       <c r="B5" t="s">
-        <v>201</v>
+        <v>187</v>
       </c>
       <c r="C5">
         <v>4</v>
@@ -4518,10 +4476,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>393</v>
+        <v>379</v>
       </c>
       <c r="B6" t="s">
-        <v>202</v>
+        <v>188</v>
       </c>
       <c r="C6">
         <v>5</v>
@@ -4548,22 +4506,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="21" t="s">
-        <v>353</v>
+      <c r="C1" s="15" t="s">
+        <v>339</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>375</v>
+        <v>361</v>
       </c>
       <c r="B2" t="s">
-        <v>374</v>
+        <v>360</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -4571,10 +4529,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>376</v>
+        <v>362</v>
       </c>
       <c r="B3" t="s">
-        <v>203</v>
+        <v>189</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -4582,10 +4540,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>377</v>
+        <v>363</v>
       </c>
       <c r="B4" t="s">
-        <v>204</v>
+        <v>190</v>
       </c>
       <c r="C4">
         <v>3</v>
@@ -4593,10 +4551,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>378</v>
+        <v>364</v>
       </c>
       <c r="B5" t="s">
-        <v>205</v>
+        <v>191</v>
       </c>
       <c r="C5">
         <v>4</v>
@@ -4622,22 +4580,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="21" t="s">
-        <v>353</v>
+      <c r="C1" s="15" t="s">
+        <v>339</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>379</v>
+        <v>365</v>
       </c>
       <c r="B2" t="s">
-        <v>206</v>
+        <v>192</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -4645,10 +4603,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>380</v>
+        <v>366</v>
       </c>
       <c r="B3" t="s">
-        <v>207</v>
+        <v>193</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -4656,10 +4614,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>381</v>
+        <v>367</v>
       </c>
       <c r="B4" t="s">
-        <v>208</v>
+        <v>194</v>
       </c>
       <c r="C4">
         <v>3</v>
@@ -4667,10 +4625,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>382</v>
+        <v>368</v>
       </c>
       <c r="B5" t="s">
-        <v>209</v>
+        <v>195</v>
       </c>
       <c r="C5">
         <v>4</v>
@@ -4678,10 +4636,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>383</v>
+        <v>369</v>
       </c>
       <c r="B6" t="s">
-        <v>210</v>
+        <v>196</v>
       </c>
       <c r="C6">
         <v>5</v>
@@ -4689,10 +4647,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>384</v>
+        <v>370</v>
       </c>
       <c r="B7" t="s">
-        <v>211</v>
+        <v>197</v>
       </c>
       <c r="C7">
         <v>6</v>
@@ -4700,10 +4658,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>385</v>
+        <v>371</v>
       </c>
       <c r="B8" t="s">
-        <v>212</v>
+        <v>198</v>
       </c>
       <c r="C8">
         <v>7</v>
@@ -4711,10 +4669,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>386</v>
+        <v>372</v>
       </c>
       <c r="B9" t="s">
-        <v>213</v>
+        <v>199</v>
       </c>
       <c r="C9">
         <v>8</v>
@@ -4722,10 +4680,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>387</v>
+        <v>373</v>
       </c>
       <c r="B10" t="s">
-        <v>433</v>
+        <v>411</v>
       </c>
       <c r="C10">
         <v>9</v>
@@ -4733,10 +4691,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>388</v>
+        <v>374</v>
       </c>
       <c r="B11" t="s">
-        <v>432</v>
+        <v>410</v>
       </c>
       <c r="C11">
         <v>10</v>
@@ -4763,22 +4721,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="21" t="s">
-        <v>353</v>
+      <c r="C1" s="15" t="s">
+        <v>339</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>354</v>
+        <v>340</v>
       </c>
       <c r="B2" t="s">
-        <v>355</v>
+        <v>341</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -4786,10 +4744,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>356</v>
+        <v>342</v>
       </c>
       <c r="B3" t="s">
-        <v>357</v>
+        <v>343</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -4797,10 +4755,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>358</v>
+        <v>344</v>
       </c>
       <c r="B4" t="s">
-        <v>359</v>
+        <v>345</v>
       </c>
       <c r="C4">
         <v>3</v>
@@ -4808,10 +4766,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>360</v>
+        <v>346</v>
       </c>
       <c r="B5" t="s">
-        <v>361</v>
+        <v>347</v>
       </c>
       <c r="C5">
         <v>4</v>
@@ -4819,10 +4777,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>362</v>
+        <v>348</v>
       </c>
       <c r="B6" t="s">
-        <v>363</v>
+        <v>349</v>
       </c>
       <c r="C6">
         <v>5</v>
@@ -4830,10 +4788,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>364</v>
+        <v>350</v>
       </c>
       <c r="B7" t="s">
-        <v>365</v>
+        <v>351</v>
       </c>
       <c r="C7">
         <v>6</v>
@@ -4841,10 +4799,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>366</v>
+        <v>352</v>
       </c>
       <c r="B8" t="s">
-        <v>367</v>
+        <v>353</v>
       </c>
       <c r="C8">
         <v>7</v>
@@ -4852,10 +4810,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>368</v>
+        <v>354</v>
       </c>
       <c r="B9" t="s">
-        <v>369</v>
+        <v>355</v>
       </c>
       <c r="C9">
         <v>8</v>
@@ -4863,10 +4821,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>370</v>
+        <v>356</v>
       </c>
       <c r="B10" t="s">
-        <v>371</v>
+        <v>357</v>
       </c>
       <c r="C10">
         <v>9</v>
@@ -4874,10 +4832,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>372</v>
+        <v>358</v>
       </c>
       <c r="B11" t="s">
-        <v>373</v>
+        <v>359</v>
       </c>
       <c r="C11">
         <v>10</v>

</xml_diff>

<commit_message>
Docs and Code Revision 251230
Moved and renamed example files 'amoniaco' to 'amonia' and 'H2SO4plant' to 'H2SO4').
- Added new example index files and updated documentation and help scripts to use new folder structure and naming conventions.
- Updated utility functions to use centralized example folder constants.
-  Added getExamplesFilename utility for easier example file path retrieval.
- Create HelpDoc folder
</commit_message>
<xml_diff>
--- a/DocUtils/Contents.xlsx
+++ b/DocUtils/Contents.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ctorr\Documents\Proyectos\TaesLab\DocUtils\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6D1B82A-2D2A-4975-B71A-9AC239BE928C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C475B61B-13B8-4429-B65C-7E9716CF8DCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3945" yWindow="780" windowWidth="12300" windowHeight="14700" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Index" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="465">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="463">
   <si>
     <t>Name</t>
   </si>
@@ -1417,12 +1417,6 @@
   </si>
   <si>
     <t>MG</t>
-  </si>
-  <si>
-    <t>fileInfo</t>
-  </si>
-  <si>
-    <t>Get information about files in a specified folder matching a pattern.</t>
   </si>
   <si>
     <t>Display a matrix using C-like formatting.</t>
@@ -1432,7 +1426,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1458,12 +1452,6 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -1483,7 +1471,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="30">
+  <borders count="29">
     <border>
       <left/>
       <right/>
@@ -1871,17 +1859,6 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
       <top style="dotted">
         <color rgb="FF000000"/>
       </top>
@@ -1894,7 +1871,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1968,9 +1945,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1989,10 +1963,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -2720,10 +2691,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:C34"/>
+  <dimension ref="A1:C33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+      <selection activeCell="A32" sqref="A32:XFD32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2737,10 +2708,10 @@
       <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="27" t="s">
+      <c r="C1" s="26" t="s">
         <v>61</v>
       </c>
     </row>
@@ -2748,7 +2719,7 @@
       <c r="A2" s="23" t="s">
         <v>327</v>
       </c>
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="28" t="s">
         <v>328</v>
       </c>
       <c r="C2" s="10">
@@ -2759,7 +2730,7 @@
       <c r="A3" s="24" t="s">
         <v>329</v>
       </c>
-      <c r="B3" s="30" t="s">
+      <c r="B3" s="29" t="s">
         <v>330</v>
       </c>
       <c r="C3" s="8">
@@ -2770,7 +2741,7 @@
       <c r="A4" s="24" t="s">
         <v>331</v>
       </c>
-      <c r="B4" s="30" t="s">
+      <c r="B4" s="29" t="s">
         <v>332</v>
       </c>
       <c r="C4" s="8">
@@ -2781,7 +2752,7 @@
       <c r="A5" s="24" t="s">
         <v>333</v>
       </c>
-      <c r="B5" s="30" t="s">
+      <c r="B5" s="29" t="s">
         <v>334</v>
       </c>
       <c r="C5" s="8">
@@ -2792,7 +2763,7 @@
       <c r="A6" s="24" t="s">
         <v>335</v>
       </c>
-      <c r="B6" s="30" t="s">
+      <c r="B6" s="29" t="s">
         <v>336</v>
       </c>
       <c r="C6" s="8">
@@ -2803,7 +2774,7 @@
       <c r="A7" s="24" t="s">
         <v>337</v>
       </c>
-      <c r="B7" s="30" t="s">
+      <c r="B7" s="29" t="s">
         <v>338</v>
       </c>
       <c r="C7" s="8">
@@ -2814,7 +2785,7 @@
       <c r="A8" s="24" t="s">
         <v>339</v>
       </c>
-      <c r="B8" s="30" t="s">
+      <c r="B8" s="29" t="s">
         <v>340</v>
       </c>
       <c r="C8" s="8">
@@ -2825,7 +2796,7 @@
       <c r="A9" s="24" t="s">
         <v>341</v>
       </c>
-      <c r="B9" s="30" t="s">
+      <c r="B9" s="29" t="s">
         <v>342</v>
       </c>
       <c r="C9" s="8">
@@ -2836,7 +2807,7 @@
       <c r="A10" s="24" t="s">
         <v>343</v>
       </c>
-      <c r="B10" s="30" t="s">
+      <c r="B10" s="29" t="s">
         <v>344</v>
       </c>
       <c r="C10" s="8">
@@ -2847,7 +2818,7 @@
       <c r="A11" s="24" t="s">
         <v>345</v>
       </c>
-      <c r="B11" s="31" t="s">
+      <c r="B11" s="30" t="s">
         <v>346</v>
       </c>
       <c r="C11" s="8">
@@ -2858,7 +2829,7 @@
       <c r="A12" s="24" t="s">
         <v>347</v>
       </c>
-      <c r="B12" s="31" t="s">
+      <c r="B12" s="30" t="s">
         <v>348</v>
       </c>
       <c r="C12" s="8">
@@ -2869,7 +2840,7 @@
       <c r="A13" s="24" t="s">
         <v>349</v>
       </c>
-      <c r="B13" s="30" t="s">
+      <c r="B13" s="29" t="s">
         <v>350</v>
       </c>
       <c r="C13" s="8">
@@ -2880,7 +2851,7 @@
       <c r="A14" s="24" t="s">
         <v>351</v>
       </c>
-      <c r="B14" s="30" t="s">
+      <c r="B14" s="29" t="s">
         <v>352</v>
       </c>
       <c r="C14" s="8">
@@ -2891,7 +2862,7 @@
       <c r="A15" s="24" t="s">
         <v>353</v>
       </c>
-      <c r="B15" s="30" t="s">
+      <c r="B15" s="29" t="s">
         <v>354</v>
       </c>
       <c r="C15" s="8">
@@ -2902,7 +2873,7 @@
       <c r="A16" s="24" t="s">
         <v>355</v>
       </c>
-      <c r="B16" s="30" t="s">
+      <c r="B16" s="29" t="s">
         <v>356</v>
       </c>
       <c r="C16" s="8">
@@ -2913,7 +2884,7 @@
       <c r="A17" s="24" t="s">
         <v>357</v>
       </c>
-      <c r="B17" s="30" t="s">
+      <c r="B17" s="29" t="s">
         <v>358</v>
       </c>
       <c r="C17" s="8">
@@ -2924,7 +2895,7 @@
       <c r="A18" s="24" t="s">
         <v>359</v>
       </c>
-      <c r="B18" s="30" t="s">
+      <c r="B18" s="29" t="s">
         <v>360</v>
       </c>
       <c r="C18" s="8">
@@ -2935,7 +2906,7 @@
       <c r="A19" s="24" t="s">
         <v>361</v>
       </c>
-      <c r="B19" s="30" t="s">
+      <c r="B19" s="29" t="s">
         <v>362</v>
       </c>
       <c r="C19" s="8">
@@ -2946,7 +2917,7 @@
       <c r="A20" s="24" t="s">
         <v>363</v>
       </c>
-      <c r="B20" s="30" t="s">
+      <c r="B20" s="29" t="s">
         <v>364</v>
       </c>
       <c r="C20" s="8">
@@ -2957,7 +2928,7 @@
       <c r="A21" s="24" t="s">
         <v>365</v>
       </c>
-      <c r="B21" s="30" t="s">
+      <c r="B21" s="29" t="s">
         <v>366</v>
       </c>
       <c r="C21" s="8">
@@ -2968,7 +2939,7 @@
       <c r="A22" s="24" t="s">
         <v>367</v>
       </c>
-      <c r="B22" s="30" t="s">
+      <c r="B22" s="29" t="s">
         <v>368</v>
       </c>
       <c r="C22" s="8">
@@ -2979,7 +2950,7 @@
       <c r="A23" s="24" t="s">
         <v>369</v>
       </c>
-      <c r="B23" s="30" t="s">
+      <c r="B23" s="29" t="s">
         <v>370</v>
       </c>
       <c r="C23" s="8">
@@ -2990,7 +2961,7 @@
       <c r="A24" s="24" t="s">
         <v>371</v>
       </c>
-      <c r="B24" s="30" t="s">
+      <c r="B24" s="29" t="s">
         <v>372</v>
       </c>
       <c r="C24" s="8">
@@ -3001,7 +2972,7 @@
       <c r="A25" s="24" t="s">
         <v>373</v>
       </c>
-      <c r="B25" s="30" t="s">
+      <c r="B25" s="29" t="s">
         <v>374</v>
       </c>
       <c r="C25" s="8">
@@ -3012,7 +2983,7 @@
       <c r="A26" s="24" t="s">
         <v>375</v>
       </c>
-      <c r="B26" s="30" t="s">
+      <c r="B26" s="29" t="s">
         <v>376</v>
       </c>
       <c r="C26" s="8">
@@ -3023,7 +2994,7 @@
       <c r="A27" s="24" t="s">
         <v>377</v>
       </c>
-      <c r="B27" s="30" t="s">
+      <c r="B27" s="29" t="s">
         <v>378</v>
       </c>
       <c r="C27" s="8">
@@ -3034,7 +3005,7 @@
       <c r="A28" s="24" t="s">
         <v>379</v>
       </c>
-      <c r="B28" s="30" t="s">
+      <c r="B28" s="29" t="s">
         <v>380</v>
       </c>
       <c r="C28" s="8">
@@ -3045,7 +3016,7 @@
       <c r="A29" s="24" t="s">
         <v>381</v>
       </c>
-      <c r="B29" s="30" t="s">
+      <c r="B29" s="29" t="s">
         <v>382</v>
       </c>
       <c r="C29" s="8">
@@ -3056,7 +3027,7 @@
       <c r="A30" s="24" t="s">
         <v>383</v>
       </c>
-      <c r="B30" s="30" t="s">
+      <c r="B30" s="29" t="s">
         <v>384</v>
       </c>
       <c r="C30" s="8">
@@ -3067,7 +3038,7 @@
       <c r="A31" s="24" t="s">
         <v>385</v>
       </c>
-      <c r="B31" s="30" t="s">
+      <c r="B31" s="29" t="s">
         <v>386</v>
       </c>
       <c r="C31" s="8">
@@ -3075,35 +3046,24 @@
       </c>
     </row>
     <row r="32" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="25" t="s">
-        <v>462</v>
-      </c>
-      <c r="B32" s="32" t="s">
-        <v>463</v>
+      <c r="A32" s="24" t="s">
+        <v>387</v>
+      </c>
+      <c r="B32" s="29" t="s">
+        <v>388</v>
       </c>
       <c r="C32" s="8">
         <v>4</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="24" t="s">
-        <v>387</v>
-      </c>
-      <c r="B33" s="30" t="s">
-        <v>388</v>
-      </c>
-      <c r="C33" s="8">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="26" t="s">
+      <c r="A33" s="25" t="s">
         <v>389</v>
       </c>
-      <c r="B34" s="33" t="s">
-        <v>464</v>
-      </c>
-      <c r="C34" s="12">
+      <c r="B33" s="31" t="s">
+        <v>462</v>
+      </c>
+      <c r="C33" s="12">
         <v>4</v>
       </c>
     </row>

</xml_diff>